<commit_message>
Problema de compatibilidade - resolvido
</commit_message>
<xml_diff>
--- a/Planilha_de_preços.xlsx
+++ b/Planilha_de_preços.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -612,22 +612,44 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>HD SSD Kingston SA400S37 480GB</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>HD SSD Kingston SA400S37 480GB</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
         <is>
           <t>223,90</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="1" t="inlineStr">
         <is>
           <t>06/03/2025 - 23:51:41</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/HD-SSD-KINGSTON-SA400S37-480GB/dp/B075BKXSCQ/ref=sr_1_3?crid=3ABFVIMZS2O0T&amp;dib=eyJ2IjoiMSJ9.xtLqN2YY2lmra89PEqy7G0Y84YkphyyUWV5twVivkNse1ODjkVlE7xfYt0-FIma8U9i0nv0Se2nMSPd-hyWG2Teo__6mPZ9JRy8ISaS7yBPhkUYWYTAJopOQ4hRMxZ7dzQoHYb3lI3LHfw_YRtgQrv4Fwxhs4tWHKz4EMr7VTkiSDRSWgvk3N6BZT1FtUAJMQc6JscsuzwuHCoTXPfmZm36OgM4cVt-aZFb9XNsALKZBTBNEIumTM7NwH3bVuyT-z9NAVFNpSltZOaTQnUckcRMTscf3YKI2hCTLpSqWQig.WagU7fhpIkWdmNgtfShtJccPMhTWlh9y46wTOG-nbZY&amp;dib_tag=se&amp;keywords=ssd+500gb&amp;qid=1732729870&amp;sprefix=ssd%2Caps%2C160&amp;sr=8-3&amp;ufe=app_do%3Aamzn1.fos.6a09f7ec-d911-4889-ad70-de8dd83c8a74</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>HD SSD Kingston SA400S37 480GB</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>259,98</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>08/08/2025 - 22:48:13</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>https://www.amazon.com.br/HD-SSD-KINGSTON-SA400S37-480GB/dp/B075BKXSCQ/ref=sr_1_3?crid=3ABFVIMZS2O0T&amp;dib=eyJ2IjoiMSJ9.xtLqN2YY2lmra89PEqy7G0Y84YkphyyUWV5twVivkNse1ODjkVlE7xfYt0-FIma8U9i0nv0Se2nMSPd-hyWG2Teo__6mPZ9JRy8ISaS7yBPhkUYWYTAJopOQ4hRMxZ7dzQoHYb3lI3LHfw_YRtgQrv4Fwxhs4tWHKz4EMr7VTkiSDRSWgvk3N6BZT1FtUAJMQc6JscsuzwuHCoTXPfmZm36OgM4cVt-aZFb9XNsALKZBTBNEIumTM7NwH3bVuyT-z9NAVFNpSltZOaTQnUckcRMTscf3YKI2hCTLpSqWQig.WagU7fhpIkWdmNgtfShtJccPMhTWlh9y46wTOG-nbZY&amp;dib_tag=se&amp;keywords=ssd+500gb&amp;qid=1732729870&amp;sprefix=ssd%2Caps%2C160&amp;sr=8-3&amp;ufe=app_do%3Aamzn1.fos.6a09f7ec-d911-4889-ad70-de8dd83c8a74</t>
         </is>

</xml_diff>